<commit_message>
Update for final paper version
</commit_message>
<xml_diff>
--- a/Analysis/Factor Details.xlsx
+++ b/Analysis/Factor Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tij.fi\Dropbox (CBS)\International Factors\Code\global-replication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tij.fi\Dropbox (CBS)\International Stock Data\Public\GlobalFactor\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3683,9 +3683,6 @@
     <t>z_score</t>
   </si>
   <si>
-    <t>intrinsic_value</t>
-  </si>
-  <si>
     <t>emp_gr1</t>
   </si>
   <si>
@@ -4566,6 +4563,9 @@
   </si>
   <si>
     <t>abr_jkp</t>
+  </si>
+  <si>
+    <t>ival_me</t>
   </si>
 </sst>
 </file>
@@ -5411,7 +5411,7 @@
   <dimension ref="A1:O256"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5427,16 +5427,16 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>601</v>
@@ -5454,22 +5454,22 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>774</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D2" t="s">
         <v>678</v>
@@ -5495,13 +5495,13 @@
         <v>7</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="K2" s="4">
         <v>9.11</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
@@ -5536,13 +5536,13 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="K3">
         <v>4.25</v>
       </c>
       <c r="L3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -5574,13 +5574,13 @@
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="K4">
         <v>3.1</v>
       </c>
       <c r="L4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -5597,7 +5597,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D5" t="s">
         <v>604</v>
@@ -5612,13 +5612,13 @@
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="K5">
         <v>2.29</v>
       </c>
       <c r="L5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -5638,7 +5638,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D6" t="s">
         <v>605</v>
@@ -5653,13 +5653,13 @@
         <v>7</v>
       </c>
       <c r="J6" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="K6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -5694,13 +5694,13 @@
         <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="K7">
         <v>2.08</v>
       </c>
       <c r="L7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -5717,7 +5717,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D8" t="s">
         <v>679</v>
@@ -5732,13 +5732,13 @@
         <v>7</v>
       </c>
       <c r="J8" t="s">
+        <v>781</v>
+      </c>
+      <c r="K8" t="s">
+        <v>776</v>
+      </c>
+      <c r="L8" t="s">
         <v>782</v>
-      </c>
-      <c r="K8" t="s">
-        <v>777</v>
-      </c>
-      <c r="L8" t="s">
-        <v>783</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -5764,7 +5764,7 @@
         <v>606</v>
       </c>
       <c r="G9" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -5773,13 +5773,13 @@
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K9">
         <v>6.42</v>
       </c>
       <c r="L9" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -5814,16 +5814,16 @@
         <v>7</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="O10" s="4">
         <v>0</v>
@@ -5843,7 +5843,7 @@
         <v>657</v>
       </c>
       <c r="G11" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="H11">
         <v>3</v>
@@ -5852,13 +5852,13 @@
         <v>7</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M11" s="4">
         <v>1</v>
@@ -5878,10 +5878,10 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D12" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G12" t="s">
         <v>34</v>
@@ -5893,13 +5893,13 @@
         <v>7</v>
       </c>
       <c r="J12" t="s">
+        <v>785</v>
+      </c>
+      <c r="K12" t="s">
         <v>786</v>
       </c>
-      <c r="K12" t="s">
-        <v>787</v>
-      </c>
       <c r="L12" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -5919,10 +5919,10 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D13" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
@@ -5934,10 +5934,10 @@
         <v>7</v>
       </c>
       <c r="J13" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="K13" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L13" s="5">
         <v>0.65</v>
@@ -5960,10 +5960,10 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D14" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G14" t="s">
         <v>37</v>
@@ -5975,10 +5975,10 @@
         <v>7</v>
       </c>
       <c r="J14" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="K14" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L14" s="5">
         <v>0.59</v>
@@ -6016,13 +6016,13 @@
         <v>7</v>
       </c>
       <c r="J15" t="s">
+        <v>788</v>
+      </c>
+      <c r="K15" t="s">
         <v>789</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>790</v>
-      </c>
-      <c r="L15" t="s">
-        <v>791</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -6054,13 +6054,13 @@
         <v>7</v>
       </c>
       <c r="J16" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="K16">
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -6092,13 +6092,13 @@
         <v>7</v>
       </c>
       <c r="J17" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="K17">
         <v>5.61</v>
       </c>
       <c r="L17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -6130,13 +6130,13 @@
         <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K18">
         <v>2.2599999999999998</v>
       </c>
       <c r="L18" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -6168,13 +6168,13 @@
         <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="K19">
         <v>5.03</v>
       </c>
       <c r="L19" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -6206,13 +6206,13 @@
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="K20">
         <v>4.1100000000000003</v>
       </c>
       <c r="L20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -6244,13 +6244,13 @@
         <v>59</v>
       </c>
       <c r="J21" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K21" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -6285,13 +6285,13 @@
         <v>59</v>
       </c>
       <c r="J22" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="K22" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -6349,13 +6349,13 @@
         <v>59</v>
       </c>
       <c r="J24" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="K24">
         <v>3.93</v>
       </c>
       <c r="L24" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -6416,13 +6416,13 @@
         <v>59</v>
       </c>
       <c r="J26" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K26">
         <v>4.28</v>
       </c>
       <c r="L26" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -6483,13 +6483,13 @@
         <v>59</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="K28" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L28" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M28">
         <v>-1</v>
@@ -6524,13 +6524,13 @@
         <v>59</v>
       </c>
       <c r="J29" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="K29" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L29" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -6591,13 +6591,13 @@
         <v>59</v>
       </c>
       <c r="J31" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="K31">
         <v>3.4</v>
       </c>
       <c r="L31" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -6614,10 +6614,10 @@
         <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D32" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G32" t="s">
         <v>90</v>
@@ -6629,13 +6629,13 @@
         <v>59</v>
       </c>
       <c r="J32" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K32" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L32" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -6693,13 +6693,13 @@
         <v>59</v>
       </c>
       <c r="J34" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="K34">
         <v>8.7899999999999991</v>
       </c>
       <c r="L34" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M34">
         <v>1</v>
@@ -6752,7 +6752,7 @@
         <v>615</v>
       </c>
       <c r="G36" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -6761,13 +6761,13 @@
         <v>59</v>
       </c>
       <c r="J36" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K36">
         <v>2.2400000000000002</v>
       </c>
       <c r="L36" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -6819,7 +6819,7 @@
         <v>616</v>
       </c>
       <c r="G38" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -6828,13 +6828,13 @@
         <v>59</v>
       </c>
       <c r="J38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K38">
         <v>4.1399999999999997</v>
       </c>
       <c r="L38" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M38">
         <v>1</v>
@@ -6880,7 +6880,7 @@
         <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>693</v>
@@ -6895,13 +6895,13 @@
         <v>59</v>
       </c>
       <c r="J40" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="K40">
         <v>-2.125</v>
       </c>
       <c r="L40" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M40">
         <v>-1</v>
@@ -6921,7 +6921,7 @@
         <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D41" t="s">
         <v>617</v>
@@ -6936,13 +6936,13 @@
         <v>59</v>
       </c>
       <c r="J41" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="K41" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M41">
         <v>-1</v>
@@ -6962,7 +6962,7 @@
         <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D42" t="s">
         <v>618</v>
@@ -6977,13 +6977,13 @@
         <v>59</v>
       </c>
       <c r="J42" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="K42">
         <v>3.08</v>
       </c>
       <c r="L42" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -7029,7 +7029,7 @@
         <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D44" t="s">
         <v>619</v>
@@ -7044,13 +7044,13 @@
         <v>59</v>
       </c>
       <c r="J44" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K44">
         <v>2.21</v>
       </c>
       <c r="L44" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M44">
         <v>1</v>
@@ -7096,13 +7096,13 @@
         <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D46" t="s">
         <v>613</v>
       </c>
       <c r="G46" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -7111,13 +7111,13 @@
         <v>59</v>
       </c>
       <c r="J46" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="K46">
         <v>8.36</v>
       </c>
       <c r="L46" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M46">
         <v>1</v>
@@ -7178,13 +7178,13 @@
         <v>59</v>
       </c>
       <c r="J48" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K48">
         <v>-4.5599999999999996</v>
       </c>
       <c r="L48" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M48">
         <v>-1</v>
@@ -7204,7 +7204,7 @@
         <v>130</v>
       </c>
       <c r="D49" t="s">
-        <v>698</v>
+        <v>992</v>
       </c>
       <c r="G49" t="s">
         <v>131</v>
@@ -7216,7 +7216,7 @@
         <v>59</v>
       </c>
       <c r="J49" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="M49">
         <v>1</v>
@@ -7248,13 +7248,13 @@
         <v>59</v>
       </c>
       <c r="J50" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K50" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L50" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -7271,7 +7271,7 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D51" t="s">
         <v>620</v>
@@ -7286,13 +7286,13 @@
         <v>59</v>
       </c>
       <c r="J51" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K51">
         <v>4.2</v>
       </c>
       <c r="L51" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M51">
         <v>1</v>
@@ -7341,7 +7341,7 @@
         <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G53" t="s">
         <v>137</v>
@@ -7353,13 +7353,13 @@
         <v>59</v>
       </c>
       <c r="J53" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K53">
         <v>-3.12</v>
       </c>
       <c r="L53" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M53">
         <v>-1</v>
@@ -7420,13 +7420,13 @@
         <v>59</v>
       </c>
       <c r="J55" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="K55">
         <v>4.63</v>
       </c>
       <c r="L55" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M55">
         <v>-1</v>
@@ -7461,13 +7461,13 @@
         <v>59</v>
       </c>
       <c r="J56" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="K56">
         <v>-4.1901999999999999</v>
       </c>
       <c r="L56" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M56">
         <v>-1</v>
@@ -7522,13 +7522,13 @@
         <v>154</v>
       </c>
       <c r="J58" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K58">
         <v>-2.76</v>
       </c>
       <c r="L58" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M58">
         <v>-1</v>
@@ -7548,7 +7548,7 @@
         <v>156</v>
       </c>
       <c r="C59" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D59" t="s">
         <v>621</v>
@@ -7563,13 +7563,13 @@
         <v>154</v>
       </c>
       <c r="J59" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K59">
         <v>-5.04</v>
       </c>
       <c r="L59" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M59">
         <v>-1</v>
@@ -7615,7 +7615,7 @@
         <v>162</v>
       </c>
       <c r="C61" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D61" t="s">
         <v>660</v>
@@ -7630,13 +7630,13 @@
         <v>154</v>
       </c>
       <c r="J61" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="K61" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L61" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M61">
         <v>-1</v>
@@ -7671,13 +7671,13 @@
         <v>154</v>
       </c>
       <c r="J62" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="K62">
         <v>-4.04</v>
       </c>
       <c r="L62" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M62">
         <v>-1</v>
@@ -7712,13 +7712,13 @@
         <v>154</v>
       </c>
       <c r="J63" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="K63">
         <v>0.17</v>
       </c>
       <c r="L63" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="M63">
         <v>-1</v>
@@ -7753,13 +7753,13 @@
         <v>154</v>
       </c>
       <c r="J64" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="K64" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L64" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M64">
         <v>-1</v>
@@ -7779,7 +7779,7 @@
         <v>173</v>
       </c>
       <c r="C65" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D65" t="s">
         <v>662</v>
@@ -7794,13 +7794,13 @@
         <v>154</v>
       </c>
       <c r="J65" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K65" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L65" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M65">
         <v>-1</v>
@@ -7820,7 +7820,7 @@
         <v>176</v>
       </c>
       <c r="C66" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D66" t="s">
         <v>664</v>
@@ -7835,13 +7835,13 @@
         <v>154</v>
       </c>
       <c r="J66" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="K66">
         <v>-5.51</v>
       </c>
       <c r="L66" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M66">
         <v>-1</v>
@@ -7861,7 +7861,7 @@
         <v>179</v>
       </c>
       <c r="C67" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D67" t="s">
         <v>663</v>
@@ -7876,13 +7876,13 @@
         <v>154</v>
       </c>
       <c r="J67" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="K67">
         <v>-5.34</v>
       </c>
       <c r="L67" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M67">
         <v>-1</v>
@@ -7917,13 +7917,13 @@
         <v>154</v>
       </c>
       <c r="J68" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K68">
         <v>-6.72</v>
       </c>
       <c r="L68" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M68">
         <v>-1</v>
@@ -7959,13 +7959,13 @@
       </c>
       <c r="J69" s="4"/>
       <c r="K69" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="O69" s="4">
         <v>0</v>
@@ -7979,7 +7979,7 @@
         <v>187</v>
       </c>
       <c r="C70" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D70" t="s">
         <v>623</v>
@@ -7994,13 +7994,13 @@
         <v>154</v>
       </c>
       <c r="J70" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K70">
         <v>-4.16</v>
       </c>
       <c r="L70" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M70">
         <v>1</v>
@@ -8020,7 +8020,7 @@
         <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D71" t="s">
         <v>624</v>
@@ -8035,13 +8035,13 @@
         <v>154</v>
       </c>
       <c r="J71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="K71">
         <v>-5.91</v>
       </c>
       <c r="L71" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M71">
         <v>-1</v>
@@ -8076,13 +8076,13 @@
         <v>154</v>
       </c>
       <c r="J72" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K72">
         <v>6.64</v>
       </c>
       <c r="L72" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M72">
         <v>-1</v>
@@ -8102,7 +8102,7 @@
         <v>194</v>
       </c>
       <c r="C73" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D73" t="s">
         <v>625</v>
@@ -8117,13 +8117,13 @@
         <v>154</v>
       </c>
       <c r="J73" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="K73" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L73" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M73">
         <v>-1</v>
@@ -8158,13 +8158,13 @@
         <v>154</v>
       </c>
       <c r="J74" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="K74" s="2">
         <v>-6.15</v>
       </c>
       <c r="L74" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M74">
         <v>-1</v>
@@ -8199,13 +8199,13 @@
         <v>154</v>
       </c>
       <c r="J75" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K75" s="2">
         <v>-6.38</v>
       </c>
       <c r="L75" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M75">
         <v>-1</v>
@@ -8225,7 +8225,7 @@
         <v>203</v>
       </c>
       <c r="C76" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>655</v>
@@ -8242,13 +8242,13 @@
         <v>154</v>
       </c>
       <c r="J76" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K76" s="2">
         <v>-8.7200000000000006</v>
       </c>
       <c r="L76" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M76">
         <v>-1</v>
@@ -8285,13 +8285,13 @@
         <v>154</v>
       </c>
       <c r="J77" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K77" s="2">
         <v>-8.7100000000000009</v>
       </c>
       <c r="L77" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M77">
         <v>-1</v>
@@ -8328,13 +8328,13 @@
         <v>154</v>
       </c>
       <c r="J78" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K78" s="2">
         <v>-4.49</v>
       </c>
       <c r="L78" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M78">
         <v>-1</v>
@@ -8371,13 +8371,13 @@
         <v>154</v>
       </c>
       <c r="J79" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K79" s="2">
         <v>-8.76</v>
       </c>
       <c r="L79" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M79">
         <v>-1</v>
@@ -8414,13 +8414,13 @@
         <v>154</v>
       </c>
       <c r="J80" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K80" s="2">
         <v>-8.44</v>
       </c>
       <c r="L80" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M80">
         <v>-1</v>
@@ -8457,13 +8457,13 @@
         <v>154</v>
       </c>
       <c r="J81" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K81" s="2">
         <v>-0.65</v>
       </c>
       <c r="L81" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M81">
         <v>-1</v>
@@ -8500,13 +8500,13 @@
         <v>154</v>
       </c>
       <c r="J82" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K82" s="2">
         <v>5.85</v>
       </c>
       <c r="L82" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M82">
         <v>1</v>
@@ -8543,13 +8543,13 @@
         <v>154</v>
       </c>
       <c r="J83" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K83" s="2">
         <v>0.43</v>
       </c>
       <c r="L83" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M83">
         <v>1</v>
@@ -8586,13 +8586,13 @@
         <v>154</v>
       </c>
       <c r="J84" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K84" s="2">
         <v>-3.38</v>
       </c>
       <c r="L84" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M84">
         <v>-1</v>
@@ -8629,13 +8629,13 @@
         <v>154</v>
       </c>
       <c r="J85" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K85" s="2">
         <v>-8.01</v>
       </c>
       <c r="L85" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M85">
         <v>-1</v>
@@ -8672,13 +8672,13 @@
         <v>154</v>
       </c>
       <c r="J86" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K86">
         <v>-6.25</v>
       </c>
       <c r="L86" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M86">
         <v>-1</v>
@@ -8713,13 +8713,13 @@
         <v>154</v>
       </c>
       <c r="J87" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="K87">
         <v>8.43</v>
       </c>
       <c r="L87" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M87">
         <v>-1</v>
@@ -8751,13 +8751,13 @@
         <v>154</v>
       </c>
       <c r="J88" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="K88" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L88" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M88">
         <v>-1</v>
@@ -8780,7 +8780,7 @@
         <v>230</v>
       </c>
       <c r="D89" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G89" t="s">
         <v>228</v>
@@ -8792,13 +8792,13 @@
         <v>154</v>
       </c>
       <c r="J89" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="K89" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L89" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M89">
         <v>-1</v>
@@ -8841,13 +8841,13 @@
         <v>234</v>
       </c>
       <c r="C91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D91" t="s">
         <v>637</v>
       </c>
       <c r="G91" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -8856,13 +8856,13 @@
         <v>154</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K91">
         <v>-5.7</v>
       </c>
       <c r="L91" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M91">
         <v>-1</v>
@@ -8882,13 +8882,13 @@
         <v>236</v>
       </c>
       <c r="C92" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D92" t="s">
         <v>638</v>
       </c>
       <c r="G92" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -8897,13 +8897,13 @@
         <v>154</v>
       </c>
       <c r="J92" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K92">
         <v>-3.2</v>
       </c>
       <c r="L92" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M92">
         <v>-1</v>
@@ -8923,13 +8923,13 @@
         <v>238</v>
       </c>
       <c r="C93" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D93" t="s">
         <v>639</v>
       </c>
       <c r="G93" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -8938,13 +8938,13 @@
         <v>154</v>
       </c>
       <c r="J93" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K93">
         <v>-8.4</v>
       </c>
       <c r="L93" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M93">
         <v>-1</v>
@@ -8964,7 +8964,7 @@
         <v>240</v>
       </c>
       <c r="C94" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D94" t="s">
         <v>667</v>
@@ -8979,13 +8979,13 @@
         <v>242</v>
       </c>
       <c r="J94" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K94">
         <v>3.11</v>
       </c>
       <c r="L94" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M94">
         <v>1</v>
@@ -9005,7 +9005,7 @@
         <v>244</v>
       </c>
       <c r="C95" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D95" t="s">
         <v>668</v>
@@ -9017,7 +9017,7 @@
         <v>242</v>
       </c>
       <c r="J95" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
@@ -9037,13 +9037,13 @@
         <v>246</v>
       </c>
       <c r="C96" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D96" t="s">
         <v>669</v>
       </c>
       <c r="G96" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="H96">
         <v>3</v>
@@ -9052,13 +9052,13 @@
         <v>242</v>
       </c>
       <c r="J96" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="K96" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M96" s="4">
         <v>1</v>
@@ -9078,7 +9078,7 @@
         <v>248</v>
       </c>
       <c r="C97" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D97" t="s">
         <v>670</v>
@@ -9090,7 +9090,7 @@
         <v>242</v>
       </c>
       <c r="J97" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
@@ -9128,13 +9128,13 @@
         <v>242</v>
       </c>
       <c r="J98" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K98">
         <v>1.41</v>
       </c>
       <c r="L98" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M98">
         <v>1</v>
@@ -9195,13 +9195,13 @@
         <v>242</v>
       </c>
       <c r="J100" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K100">
         <v>1.04</v>
       </c>
       <c r="L100" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M100">
         <v>1</v>
@@ -9265,13 +9265,13 @@
         <v>242</v>
       </c>
       <c r="J102" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K102">
         <v>0.28999999999999998</v>
       </c>
       <c r="L102" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M102">
         <v>1</v>
@@ -9335,13 +9335,13 @@
         <v>242</v>
       </c>
       <c r="J104" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="K104" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L104" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M104">
         <v>1</v>
@@ -9402,13 +9402,13 @@
         <v>242</v>
       </c>
       <c r="J106" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="K106">
         <v>4.59</v>
       </c>
       <c r="L106" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M106">
         <v>1</v>
@@ -9443,7 +9443,7 @@
         <v>242</v>
       </c>
       <c r="J107" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M107">
         <v>1</v>
@@ -9501,13 +9501,13 @@
         <v>242</v>
       </c>
       <c r="J109" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="K109">
         <v>2.92</v>
       </c>
       <c r="L109" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M109">
         <v>1</v>
@@ -9542,7 +9542,7 @@
         <v>242</v>
       </c>
       <c r="J110" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
@@ -9600,7 +9600,7 @@
         <v>242</v>
       </c>
       <c r="J112" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="M112" s="4">
         <v>1</v>
@@ -9635,13 +9635,13 @@
         <v>242</v>
       </c>
       <c r="J113" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K113">
         <v>8.86</v>
       </c>
       <c r="L113" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M113">
         <v>1</v>
@@ -9699,7 +9699,7 @@
         <v>242</v>
       </c>
       <c r="J115" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M115">
         <v>1</v>
@@ -9734,13 +9734,13 @@
         <v>242</v>
       </c>
       <c r="J116" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K116">
         <v>5.27</v>
       </c>
       <c r="L116" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M116">
         <v>1</v>
@@ -9786,13 +9786,13 @@
         <v>295</v>
       </c>
       <c r="C118" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D118" t="s">
         <v>695</v>
       </c>
       <c r="G118" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -9801,13 +9801,13 @@
         <v>242</v>
       </c>
       <c r="J118" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="K118">
         <v>5.8890000000000002</v>
       </c>
       <c r="L118" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M118">
         <v>1</v>
@@ -9905,7 +9905,7 @@
         <v>304</v>
       </c>
       <c r="C122" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D122" t="s">
         <v>696</v>
@@ -9920,13 +9920,13 @@
         <v>242</v>
       </c>
       <c r="J122" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="K122">
         <v>-3.38</v>
       </c>
       <c r="L122" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M122">
         <v>-1</v>
@@ -9972,7 +9972,7 @@
         <v>309</v>
       </c>
       <c r="C124" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D124" t="s">
         <v>697</v>
@@ -9987,13 +9987,13 @@
         <v>242</v>
       </c>
       <c r="J124" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="K124">
         <v>3.37</v>
       </c>
       <c r="L124" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M124">
         <v>1</v>
@@ -10054,13 +10054,13 @@
         <v>242</v>
       </c>
       <c r="J126" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="K126">
         <v>-2.8</v>
       </c>
       <c r="L126" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M126">
         <v>-1</v>
@@ -10092,13 +10092,13 @@
         <v>242</v>
       </c>
       <c r="J127" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="K127" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="L127" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M127">
         <v>1</v>
@@ -10159,13 +10159,13 @@
         <v>242</v>
       </c>
       <c r="J129" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="K129">
         <v>5.53</v>
       </c>
       <c r="L129" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M129">
         <v>1</v>
@@ -10197,13 +10197,13 @@
         <v>242</v>
       </c>
       <c r="J130" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K130">
         <v>-4.45</v>
       </c>
       <c r="L130" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M130">
         <v>-1</v>
@@ -10249,7 +10249,7 @@
         <v>328</v>
       </c>
       <c r="C132" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D132" t="s">
         <v>671</v>
@@ -10261,7 +10261,7 @@
         <v>242</v>
       </c>
       <c r="J132" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M132">
         <v>-1</v>
@@ -10293,13 +10293,13 @@
         <v>332</v>
       </c>
       <c r="J133" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="K133">
         <v>2.85</v>
       </c>
       <c r="L133" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M133">
         <v>1</v>
@@ -10354,13 +10354,13 @@
         <v>332</v>
       </c>
       <c r="J135" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K135" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L135" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M135">
         <v>1</v>
@@ -10392,13 +10392,13 @@
         <v>332</v>
       </c>
       <c r="J136" t="s">
+        <v>830</v>
+      </c>
+      <c r="K136" t="s">
+        <v>776</v>
+      </c>
+      <c r="L136" t="s">
         <v>831</v>
-      </c>
-      <c r="K136" t="s">
-        <v>777</v>
-      </c>
-      <c r="L136" t="s">
-        <v>832</v>
       </c>
       <c r="M136">
         <v>-1</v>
@@ -10415,13 +10415,13 @@
         <v>342</v>
       </c>
       <c r="C137" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D137" t="s">
         <v>648</v>
       </c>
       <c r="G137" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="H137">
         <v>1</v>
@@ -10430,13 +10430,13 @@
         <v>332</v>
       </c>
       <c r="J137" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K137" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L137" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M137">
         <v>1</v>
@@ -10482,13 +10482,13 @@
         <v>347</v>
       </c>
       <c r="C139" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D139" t="s">
         <v>649</v>
       </c>
       <c r="G139" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="H139">
         <v>1</v>
@@ -10497,13 +10497,13 @@
         <v>332</v>
       </c>
       <c r="J139" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K139" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L139" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M139">
         <v>1</v>
@@ -10564,13 +10564,13 @@
         <v>332</v>
       </c>
       <c r="J141" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="K141">
         <v>2.52</v>
       </c>
       <c r="L141" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M141">
         <v>1</v>
@@ -10619,7 +10619,7 @@
         <v>356</v>
       </c>
       <c r="D143" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G143" t="s">
         <v>357</v>
@@ -10631,13 +10631,13 @@
         <v>332</v>
       </c>
       <c r="J143" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="K143">
         <v>-3.09</v>
       </c>
       <c r="L143" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M143">
         <v>-1</v>
@@ -10663,7 +10663,7 @@
         <v>672</v>
       </c>
       <c r="G144" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="H144">
         <v>1</v>
@@ -10672,13 +10672,13 @@
         <v>332</v>
       </c>
       <c r="J144" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K144" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L144" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M144">
         <v>1</v>
@@ -10714,13 +10714,13 @@
       </c>
       <c r="J145" s="7"/>
       <c r="K145" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L145" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M145" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="O145">
         <v>0</v>
@@ -10749,13 +10749,13 @@
         <v>332</v>
       </c>
       <c r="J146" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="K146" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L146" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M146">
         <v>-1</v>
@@ -10787,13 +10787,13 @@
         <v>332</v>
       </c>
       <c r="J147" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K147" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L147" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M147">
         <v>-1</v>
@@ -10825,13 +10825,13 @@
         <v>332</v>
       </c>
       <c r="J148" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="K148">
         <v>1.81</v>
       </c>
       <c r="L148" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M148">
         <v>1</v>
@@ -10863,13 +10863,13 @@
         <v>332</v>
       </c>
       <c r="J149" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="K149">
         <v>2.92</v>
       </c>
       <c r="L149" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M149">
         <v>1</v>
@@ -10901,13 +10901,13 @@
         <v>332</v>
       </c>
       <c r="J150" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K150">
         <v>-2.85</v>
       </c>
       <c r="L150" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M150">
         <v>-1</v>
@@ -10939,13 +10939,13 @@
         <v>332</v>
       </c>
       <c r="J151" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K151">
         <v>-2.12</v>
       </c>
       <c r="L151" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M151">
         <v>-1</v>
@@ -10977,13 +10977,13 @@
         <v>332</v>
       </c>
       <c r="J152" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K152">
         <v>-2.2799999999999998</v>
       </c>
       <c r="L152" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M152">
         <v>-1</v>
@@ -11015,13 +11015,13 @@
         <v>332</v>
       </c>
       <c r="J153" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="K153">
         <v>-3.46</v>
       </c>
       <c r="L153" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M153">
         <v>-1</v>
@@ -11056,13 +11056,13 @@
         <v>332</v>
       </c>
       <c r="J154" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="K154">
         <v>4.37</v>
       </c>
       <c r="L154" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M154">
         <v>1</v>
@@ -11094,13 +11094,13 @@
         <v>332</v>
       </c>
       <c r="J155" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K155">
         <v>7.7</v>
       </c>
       <c r="L155" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M155">
         <v>1</v>
@@ -11132,13 +11132,13 @@
         <v>332</v>
       </c>
       <c r="J156" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K156">
         <v>7.39</v>
       </c>
       <c r="L156" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M156">
         <v>1</v>
@@ -11155,7 +11155,7 @@
         <v>392</v>
       </c>
       <c r="C157" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D157" t="s">
         <v>674</v>
@@ -11170,13 +11170,13 @@
         <v>332</v>
       </c>
       <c r="J157" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K157">
         <v>2.0630000000000002</v>
       </c>
       <c r="L157" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M157">
         <v>1</v>
@@ -11196,7 +11196,7 @@
         <v>394</v>
       </c>
       <c r="C158" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D158" t="s">
         <v>675</v>
@@ -11211,13 +11211,13 @@
         <v>332</v>
       </c>
       <c r="J158" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K158">
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="L158" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M158">
         <v>-1</v>
@@ -11237,7 +11237,7 @@
         <v>396</v>
       </c>
       <c r="C159" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D159" t="s">
         <v>676</v>
@@ -11252,13 +11252,13 @@
         <v>332</v>
       </c>
       <c r="J159" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K159">
         <v>1.304</v>
       </c>
       <c r="L159" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M159">
         <v>1</v>
@@ -11278,7 +11278,7 @@
         <v>398</v>
       </c>
       <c r="C160" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D160" t="s">
         <v>677</v>
@@ -11293,13 +11293,13 @@
         <v>332</v>
       </c>
       <c r="J160" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K160">
         <v>1.363</v>
       </c>
       <c r="L160" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M160">
         <v>1</v>
@@ -11334,13 +11334,13 @@
         <v>332</v>
       </c>
       <c r="J161" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K161">
         <v>0.11600000000000001</v>
       </c>
       <c r="L161" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M161">
         <v>1</v>
@@ -11360,7 +11360,7 @@
         <v>402</v>
       </c>
       <c r="D162" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G162" t="s">
         <v>185</v>
@@ -11372,13 +11372,13 @@
         <v>332</v>
       </c>
       <c r="J162" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K162">
         <v>1.113</v>
       </c>
       <c r="L162" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M162">
         <v>1</v>
@@ -11413,13 +11413,13 @@
         <v>332</v>
       </c>
       <c r="J163" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="K163" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L163" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M163">
         <v>1</v>
@@ -11436,7 +11436,7 @@
         <v>406</v>
       </c>
       <c r="C164" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D164" t="s">
         <v>692</v>
@@ -11451,13 +11451,13 @@
         <v>332</v>
       </c>
       <c r="J164" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K164">
         <v>5.04</v>
       </c>
       <c r="L164" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M164" s="2">
         <v>1</v>
@@ -11518,13 +11518,13 @@
         <v>332</v>
       </c>
       <c r="J166" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="K166">
         <v>1.8</v>
       </c>
       <c r="L166" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M166">
         <v>1</v>
@@ -11541,10 +11541,10 @@
         <v>414</v>
       </c>
       <c r="C167" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D167" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G167" t="s">
         <v>415</v>
@@ -11556,13 +11556,13 @@
         <v>332</v>
       </c>
       <c r="J167" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="K167">
         <v>3.06</v>
       </c>
       <c r="L167" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M167">
         <v>1</v>
@@ -11623,13 +11623,13 @@
         <v>332</v>
       </c>
       <c r="J169" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K169">
         <v>3.17</v>
       </c>
       <c r="L169" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M169">
         <v>1</v>
@@ -11687,13 +11687,13 @@
         <v>332</v>
       </c>
       <c r="J171" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="K171" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L171" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M171">
         <v>1</v>
@@ -11725,13 +11725,13 @@
         <v>332</v>
       </c>
       <c r="J172" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="K172" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L172" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M172">
         <v>1</v>
@@ -11754,7 +11754,7 @@
         <v>691</v>
       </c>
       <c r="G173" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="H173">
         <v>3</v>
@@ -11763,13 +11763,13 @@
         <v>332</v>
       </c>
       <c r="J173" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K173">
         <v>-1.98</v>
       </c>
       <c r="L173" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M173">
         <v>-1</v>
@@ -11795,7 +11795,7 @@
         <v>651</v>
       </c>
       <c r="G174" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="H174">
         <v>3</v>
@@ -11804,13 +11804,13 @@
         <v>332</v>
       </c>
       <c r="J174" t="s">
+        <v>843</v>
+      </c>
+      <c r="K174" t="s">
         <v>844</v>
       </c>
-      <c r="K174" t="s">
-        <v>845</v>
-      </c>
       <c r="L174" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M174">
         <v>1</v>
@@ -11845,13 +11845,13 @@
         <v>332</v>
       </c>
       <c r="J175" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="K175">
         <v>0.04</v>
       </c>
       <c r="L175" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M175">
         <v>1</v>
@@ -11883,13 +11883,13 @@
         <v>332</v>
       </c>
       <c r="J176" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K176">
         <v>47.85</v>
       </c>
       <c r="L176" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M176">
         <v>1</v>
@@ -11947,13 +11947,13 @@
         <v>332</v>
       </c>
       <c r="J178" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="K178">
         <v>-2.12</v>
       </c>
       <c r="L178" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M178">
         <v>-1</v>
@@ -11973,7 +11973,7 @@
         <v>445</v>
       </c>
       <c r="D179" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G179" t="s">
         <v>446</v>
@@ -11985,13 +11985,13 @@
         <v>332</v>
       </c>
       <c r="J179" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K179" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L179" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M179">
         <v>1</v>
@@ -12011,10 +12011,10 @@
         <v>448</v>
       </c>
       <c r="C180" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D180" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G180" t="s">
         <v>446</v>
@@ -12026,13 +12026,13 @@
         <v>332</v>
       </c>
       <c r="J180" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K180" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L180" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M180">
         <v>1</v>
@@ -12052,10 +12052,10 @@
         <v>450</v>
       </c>
       <c r="C181" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D181" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F181">
         <v>1</v>
@@ -12070,13 +12070,13 @@
         <v>332</v>
       </c>
       <c r="J181" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K181" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L181" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M181">
         <v>-1</v>
@@ -12111,13 +12111,13 @@
         <v>332</v>
       </c>
       <c r="J182" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K182" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L182" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M182">
         <v>1</v>
@@ -12149,13 +12149,13 @@
         <v>332</v>
       </c>
       <c r="J183" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K183" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L183" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M183">
         <v>1</v>
@@ -12187,13 +12187,13 @@
         <v>332</v>
       </c>
       <c r="J184" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K184" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L184" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M184">
         <v>1</v>
@@ -12225,13 +12225,13 @@
         <v>332</v>
       </c>
       <c r="J185" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="K185">
         <v>2.1</v>
       </c>
       <c r="L185" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M185">
         <v>1</v>
@@ -12263,13 +12263,13 @@
         <v>332</v>
       </c>
       <c r="K186" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L186" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M186" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -12283,7 +12283,7 @@
         <v>463</v>
       </c>
       <c r="D187" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G187" t="s">
         <v>464</v>
@@ -12295,13 +12295,13 @@
         <v>332</v>
       </c>
       <c r="J187" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K187" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L187" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M187">
         <v>-1</v>
@@ -12333,10 +12333,10 @@
         <v>332</v>
       </c>
       <c r="K188" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L188" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M188">
         <v>-1</v>
@@ -12353,7 +12353,7 @@
         <v>468</v>
       </c>
       <c r="D189" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G189" t="s">
         <v>464</v>
@@ -12365,13 +12365,13 @@
         <v>332</v>
       </c>
       <c r="J189" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K189" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L189" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M189">
         <v>-1</v>
@@ -12403,10 +12403,10 @@
         <v>332</v>
       </c>
       <c r="K190" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L190" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M190">
         <v>-1</v>
@@ -12435,13 +12435,13 @@
         <v>332</v>
       </c>
       <c r="J191" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="K191">
         <v>-2.72</v>
       </c>
       <c r="L191" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M191">
         <v>1</v>
@@ -12473,13 +12473,13 @@
         <v>332</v>
       </c>
       <c r="J192" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="K192">
         <v>-2.31</v>
       </c>
       <c r="L192" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M192">
         <v>-1</v>
@@ -12511,13 +12511,13 @@
         <v>332</v>
       </c>
       <c r="J193" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="K193">
         <v>2.79</v>
       </c>
       <c r="L193" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M193">
         <v>1</v>
@@ -12537,7 +12537,7 @@
         <v>481</v>
       </c>
       <c r="D194" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G194" t="s">
         <v>482</v>
@@ -12549,13 +12549,13 @@
         <v>332</v>
       </c>
       <c r="J194" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K194">
         <v>7.6</v>
       </c>
       <c r="L194" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M194">
         <v>1</v>
@@ -12578,7 +12578,7 @@
         <v>484</v>
       </c>
       <c r="D195" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G195" t="s">
         <v>482</v>
@@ -12590,13 +12590,13 @@
         <v>332</v>
       </c>
       <c r="J195" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K195">
         <v>4.2</v>
       </c>
       <c r="L195" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M195">
         <v>1</v>
@@ -12616,10 +12616,10 @@
         <v>486</v>
       </c>
       <c r="C196" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D196" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G196" t="s">
         <v>482</v>
@@ -12631,13 +12631,13 @@
         <v>332</v>
       </c>
       <c r="J196" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K196">
         <v>5.35</v>
       </c>
       <c r="L196" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M196">
         <v>1</v>
@@ -12657,10 +12657,10 @@
         <v>488</v>
       </c>
       <c r="C197" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D197" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G197" t="s">
         <v>482</v>
@@ -12672,13 +12672,13 @@
         <v>332</v>
       </c>
       <c r="J197" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K197">
         <v>-5.6</v>
       </c>
       <c r="L197" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M197">
         <v>-1</v>
@@ -12698,10 +12698,10 @@
         <v>490</v>
       </c>
       <c r="C198" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D198" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G198" t="s">
         <v>482</v>
@@ -12713,13 +12713,13 @@
         <v>332</v>
       </c>
       <c r="J198" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K198">
         <v>6.15</v>
       </c>
       <c r="L198" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M198">
         <v>1</v>
@@ -12739,10 +12739,10 @@
         <v>492</v>
       </c>
       <c r="C199" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D199" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G199" t="s">
         <v>482</v>
@@ -12754,13 +12754,13 @@
         <v>332</v>
       </c>
       <c r="J199" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K199">
         <v>-4.62</v>
       </c>
       <c r="L199" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M199">
         <v>-1</v>
@@ -12780,10 +12780,10 @@
         <v>494</v>
       </c>
       <c r="C200" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D200" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G200" t="s">
         <v>482</v>
@@ -12795,13 +12795,13 @@
         <v>332</v>
       </c>
       <c r="J200" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K200">
         <v>6.43</v>
       </c>
       <c r="L200" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M200">
         <v>1</v>
@@ -12821,10 +12821,10 @@
         <v>496</v>
       </c>
       <c r="C201" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D201" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G201" t="s">
         <v>482</v>
@@ -12836,13 +12836,13 @@
         <v>332</v>
       </c>
       <c r="J201" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K201">
         <v>-1.77</v>
       </c>
       <c r="L201" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M201">
         <v>-1</v>
@@ -12862,10 +12862,10 @@
         <v>498</v>
       </c>
       <c r="C202" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D202" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G202" t="s">
         <v>482</v>
@@ -12877,13 +12877,13 @@
         <v>332</v>
       </c>
       <c r="J202" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K202">
         <v>4.58</v>
       </c>
       <c r="L202" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M202">
         <v>1</v>
@@ -12903,10 +12903,10 @@
         <v>500</v>
       </c>
       <c r="C203" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D203" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G203" t="s">
         <v>482</v>
@@ -12918,13 +12918,13 @@
         <v>332</v>
       </c>
       <c r="J203" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="K203">
         <v>-3.35</v>
       </c>
       <c r="L203" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M203">
         <v>-1</v>
@@ -12944,7 +12944,7 @@
         <v>502</v>
       </c>
       <c r="C204" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D204" t="s">
         <v>652</v>
@@ -12959,13 +12959,13 @@
         <v>504</v>
       </c>
       <c r="J204" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="K204">
         <v>-2.42</v>
       </c>
       <c r="L204" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M204">
         <v>-1</v>
@@ -12988,7 +12988,7 @@
         <v>506</v>
       </c>
       <c r="D205" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G205" t="s">
         <v>507</v>
@@ -13000,13 +13000,13 @@
         <v>504</v>
       </c>
       <c r="J205" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="K205">
         <v>-2.86</v>
       </c>
       <c r="L205" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M205">
         <v>-1</v>
@@ -13026,10 +13026,10 @@
         <v>509</v>
       </c>
       <c r="C206" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D206" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G206" t="s">
         <v>510</v>
@@ -13041,13 +13041,13 @@
         <v>504</v>
       </c>
       <c r="J206" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="K206">
         <v>-2.69</v>
       </c>
       <c r="L206" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M206">
         <v>-1</v>
@@ -13067,10 +13067,10 @@
         <v>511</v>
       </c>
       <c r="C207" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D207" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H207">
         <v>3</v>
@@ -13079,7 +13079,7 @@
         <v>504</v>
       </c>
       <c r="J207" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M207">
         <v>-1</v>
@@ -13099,7 +13099,7 @@
         <v>513</v>
       </c>
       <c r="D208" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H208">
         <v>3</v>
@@ -13108,7 +13108,7 @@
         <v>504</v>
       </c>
       <c r="J208" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M208">
         <v>-1</v>
@@ -13125,7 +13125,7 @@
         <v>515</v>
       </c>
       <c r="C209" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D209" t="s">
         <v>656</v>
@@ -13140,13 +13140,13 @@
         <v>504</v>
       </c>
       <c r="J209" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="K209">
         <v>-2.86</v>
       </c>
       <c r="L209" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M209">
         <v>-1</v>
@@ -13181,10 +13181,10 @@
         <v>504</v>
       </c>
       <c r="K210" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L210" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M210">
         <v>-1</v>
@@ -13201,7 +13201,7 @@
         <v>520</v>
       </c>
       <c r="C211" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D211" t="s">
         <v>653</v>
@@ -13216,13 +13216,13 @@
         <v>504</v>
       </c>
       <c r="J211" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="K211">
         <v>1.85</v>
       </c>
       <c r="L211" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M211">
         <v>-1</v>
@@ -13242,10 +13242,10 @@
         <v>523</v>
       </c>
       <c r="C212" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D212" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G212" t="s">
         <v>524</v>
@@ -13257,13 +13257,13 @@
         <v>504</v>
       </c>
       <c r="J212" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="K212">
         <v>7.12</v>
       </c>
       <c r="L212" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M212">
         <v>-1</v>
@@ -13283,10 +13283,10 @@
         <v>526</v>
       </c>
       <c r="C213" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D213" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G213" t="s">
         <v>527</v>
@@ -13298,13 +13298,13 @@
         <v>504</v>
       </c>
       <c r="J213" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="K213" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L213" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M213">
         <v>-1</v>
@@ -13327,7 +13327,7 @@
         <v>529</v>
       </c>
       <c r="D214" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G214" t="s">
         <v>530</v>
@@ -13339,13 +13339,13 @@
         <v>504</v>
       </c>
       <c r="J214" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="K214">
         <v>-8.58</v>
       </c>
       <c r="L214" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M214">
         <v>-1</v>
@@ -13368,7 +13368,7 @@
         <v>532</v>
       </c>
       <c r="D215" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G215" t="s">
         <v>533</v>
@@ -13380,13 +13380,13 @@
         <v>504</v>
       </c>
       <c r="J215" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="K215">
         <v>-6.03</v>
       </c>
       <c r="L215" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M215">
         <v>-1</v>
@@ -13409,7 +13409,7 @@
         <v>535</v>
       </c>
       <c r="D216" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G216" t="s">
         <v>536</v>
@@ -13421,13 +13421,13 @@
         <v>504</v>
       </c>
       <c r="J216" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="K216">
         <v>2.86</v>
       </c>
       <c r="L216" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M216">
         <v>-1</v>
@@ -13450,7 +13450,7 @@
         <v>538</v>
       </c>
       <c r="D217" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G217" t="s">
         <v>533</v>
@@ -13462,13 +13462,13 @@
         <v>504</v>
       </c>
       <c r="J217" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="K217">
         <v>-5.0999999999999996</v>
       </c>
       <c r="L217" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M217">
         <v>-1</v>
@@ -13503,13 +13503,13 @@
         <v>504</v>
       </c>
       <c r="J218" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="K218">
         <v>3</v>
       </c>
       <c r="L218" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M218">
         <v>-1</v>
@@ -13529,10 +13529,10 @@
         <v>543</v>
       </c>
       <c r="C219" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D219" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G219" t="s">
         <v>544</v>
@@ -13544,13 +13544,13 @@
         <v>504</v>
       </c>
       <c r="J219" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="K219">
         <v>5.39</v>
       </c>
       <c r="L219" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M219">
         <v>1</v>
@@ -13570,10 +13570,10 @@
         <v>546</v>
       </c>
       <c r="C220" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D220" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G220" t="s">
         <v>547</v>
@@ -13585,13 +13585,13 @@
         <v>504</v>
       </c>
       <c r="J220" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="K220">
         <v>0.93</v>
       </c>
       <c r="L220" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M220">
         <v>1</v>
@@ -13611,10 +13611,10 @@
         <v>549</v>
       </c>
       <c r="C221" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D221" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G221" t="s">
         <v>547</v>
@@ -13626,13 +13626,13 @@
         <v>504</v>
       </c>
       <c r="J221" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="K221">
         <v>4.0599999999999996</v>
       </c>
       <c r="L221" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M221">
         <v>1</v>
@@ -13652,10 +13652,10 @@
         <v>551</v>
       </c>
       <c r="C222" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D222" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G222" t="s">
         <v>547</v>
@@ -13667,13 +13667,13 @@
         <v>504</v>
       </c>
       <c r="J222" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="K222">
         <v>4.4000000000000004</v>
       </c>
       <c r="L222" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M222">
         <v>1</v>
@@ -13696,7 +13696,7 @@
         <v>553</v>
       </c>
       <c r="D223" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G223" t="s">
         <v>554</v>
@@ -13708,13 +13708,13 @@
         <v>504</v>
       </c>
       <c r="J223" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="K223">
         <v>-6.16</v>
       </c>
       <c r="L223" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M223">
         <v>-1</v>
@@ -13737,7 +13737,7 @@
         <v>556</v>
       </c>
       <c r="D224" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G224" t="s">
         <v>557</v>
@@ -13749,13 +13749,13 @@
         <v>504</v>
       </c>
       <c r="J224" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="K224">
         <v>-4.01</v>
       </c>
       <c r="L224" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M224">
         <v>-1</v>
@@ -13778,7 +13778,7 @@
         <v>559</v>
       </c>
       <c r="D225" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H225">
         <v>3</v>
@@ -13787,7 +13787,7 @@
         <v>504</v>
       </c>
       <c r="J225" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M225" s="8">
         <v>-1</v>
@@ -13807,7 +13807,7 @@
         <v>561</v>
       </c>
       <c r="D226" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G226" t="s">
         <v>557</v>
@@ -13819,13 +13819,13 @@
         <v>504</v>
       </c>
       <c r="J226" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="K226">
         <v>-2.44</v>
       </c>
       <c r="L226" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M226">
         <v>-1</v>
@@ -13848,7 +13848,7 @@
         <v>563</v>
       </c>
       <c r="D227" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H227">
         <v>3</v>
@@ -13857,7 +13857,7 @@
         <v>504</v>
       </c>
       <c r="J227" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M227" s="8">
         <v>-1</v>
@@ -13877,7 +13877,7 @@
         <v>565</v>
       </c>
       <c r="D228" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G228" t="s">
         <v>566</v>
@@ -13889,13 +13889,13 @@
         <v>504</v>
       </c>
       <c r="J228" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K228" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L228" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M228">
         <v>-1</v>
@@ -13930,13 +13930,13 @@
         <v>504</v>
       </c>
       <c r="J229" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="K229">
         <v>2.12</v>
       </c>
       <c r="L229" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M229">
         <v>1</v>
@@ -13968,13 +13968,13 @@
         <v>504</v>
       </c>
       <c r="J230" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K230">
         <v>0.46800000000000003</v>
       </c>
       <c r="L230" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M230">
         <v>1</v>
@@ -14006,13 +14006,13 @@
         <v>504</v>
       </c>
       <c r="J231" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K231">
         <v>-0.28000000000000003</v>
       </c>
       <c r="L231" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M231">
         <v>-1</v>
@@ -14044,13 +14044,13 @@
         <v>504</v>
       </c>
       <c r="J232" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K232">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="L232" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M232">
         <v>1</v>
@@ -14082,13 +14082,13 @@
         <v>504</v>
       </c>
       <c r="J233" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K233">
         <v>-1.1299999999999999</v>
       </c>
       <c r="L233" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M233">
         <v>-1</v>
@@ -14120,13 +14120,13 @@
         <v>504</v>
       </c>
       <c r="J234" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K234">
         <v>2.532</v>
       </c>
       <c r="L234" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M234">
         <v>1</v>
@@ -14146,7 +14146,7 @@
         <v>582</v>
       </c>
       <c r="D235" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G235" t="s">
         <v>583</v>
@@ -14158,13 +14158,13 @@
         <v>504</v>
       </c>
       <c r="J235" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="K235">
         <v>-18.579999999999998</v>
       </c>
       <c r="L235" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M235">
         <v>-1</v>
@@ -14187,7 +14187,7 @@
         <v>585</v>
       </c>
       <c r="D236" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="G236" t="s">
         <v>586</v>
@@ -14199,13 +14199,13 @@
         <v>504</v>
       </c>
       <c r="J236" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K236">
         <v>5.25</v>
       </c>
       <c r="L236" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M236" s="8">
         <v>-1</v>
@@ -14228,7 +14228,7 @@
         <v>588</v>
       </c>
       <c r="D237" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G237" t="s">
         <v>589</v>
@@ -14240,13 +14240,13 @@
         <v>504</v>
       </c>
       <c r="J237" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K237">
         <v>12.78</v>
       </c>
       <c r="L237" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M237">
         <v>1</v>
@@ -14281,13 +14281,13 @@
         <v>504</v>
       </c>
       <c r="J238" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K238">
         <v>1.26</v>
       </c>
       <c r="L238" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M238">
         <v>1</v>
@@ -14319,13 +14319,13 @@
         <v>504</v>
       </c>
       <c r="J239" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="K239" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L239" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M239">
         <v>1</v>
@@ -14360,7 +14360,7 @@
         <v>2.37</v>
       </c>
       <c r="L240" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M240">
         <v>1</v>
@@ -14389,13 +14389,13 @@
         <v>504</v>
       </c>
       <c r="J241" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="K241">
         <v>2.496</v>
       </c>
       <c r="L241" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="M241">
         <v>1</v>
@@ -14406,22 +14406,22 @@
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
+        <v>736</v>
+      </c>
+      <c r="C242" t="s">
+        <v>974</v>
+      </c>
+      <c r="D242" t="s">
         <v>737</v>
       </c>
-      <c r="C242" t="s">
-        <v>975</v>
-      </c>
-      <c r="D242" t="s">
-        <v>738</v>
-      </c>
       <c r="G242" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I242" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J242" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="M242">
         <v>1</v>
@@ -14432,22 +14432,22 @@
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
+        <v>738</v>
+      </c>
+      <c r="C243" t="s">
+        <v>975</v>
+      </c>
+      <c r="D243" t="s">
         <v>739</v>
       </c>
-      <c r="C243" t="s">
-        <v>976</v>
-      </c>
-      <c r="D243" t="s">
-        <v>740</v>
-      </c>
       <c r="G243" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I243" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J243" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="M243">
         <v>1</v>
@@ -14458,22 +14458,22 @@
     </row>
     <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
+        <v>740</v>
+      </c>
+      <c r="C244" t="s">
+        <v>976</v>
+      </c>
+      <c r="D244" t="s">
         <v>741</v>
       </c>
-      <c r="C244" t="s">
-        <v>977</v>
-      </c>
-      <c r="D244" t="s">
-        <v>742</v>
-      </c>
       <c r="G244" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I244" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J244" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="M244">
         <v>1</v>
@@ -14484,22 +14484,22 @@
     </row>
     <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
+        <v>745</v>
+      </c>
+      <c r="C245" t="s">
+        <v>977</v>
+      </c>
+      <c r="D245" t="s">
+        <v>744</v>
+      </c>
+      <c r="G245" t="s">
         <v>746</v>
       </c>
-      <c r="C245" t="s">
-        <v>978</v>
-      </c>
-      <c r="D245" t="s">
-        <v>745</v>
-      </c>
-      <c r="G245" t="s">
-        <v>747</v>
-      </c>
       <c r="I245" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J245" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="M245">
         <v>-1</v>
@@ -14510,22 +14510,22 @@
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
+        <v>747</v>
+      </c>
+      <c r="C246" t="s">
+        <v>747</v>
+      </c>
+      <c r="D246" t="s">
         <v>748</v>
       </c>
-      <c r="C246" t="s">
-        <v>748</v>
-      </c>
-      <c r="D246" t="s">
-        <v>749</v>
-      </c>
       <c r="G246" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I246" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J246" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="M246">
         <v>-1</v>
@@ -14536,22 +14536,22 @@
     </row>
     <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C247" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D247" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G247" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I247" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J247" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="M247">
         <v>-1</v>
@@ -14562,22 +14562,22 @@
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C248" t="s">
         <v>240</v>
       </c>
       <c r="D248" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G248" t="s">
         <v>264</v>
       </c>
       <c r="I248" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J248" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="M248">
         <v>1</v>
@@ -14588,22 +14588,22 @@
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
+        <v>755</v>
+      </c>
+      <c r="C249" t="s">
+        <v>755</v>
+      </c>
+      <c r="D249" t="s">
         <v>756</v>
       </c>
-      <c r="C249" t="s">
-        <v>756</v>
-      </c>
-      <c r="D249" t="s">
-        <v>757</v>
-      </c>
       <c r="G249" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I249" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J249" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M249">
         <v>1</v>
@@ -14614,22 +14614,22 @@
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
+        <v>757</v>
+      </c>
+      <c r="C250" t="s">
+        <v>978</v>
+      </c>
+      <c r="D250" t="s">
+        <v>768</v>
+      </c>
+      <c r="G250" t="s">
         <v>758</v>
       </c>
-      <c r="C250" t="s">
-        <v>979</v>
-      </c>
-      <c r="D250" t="s">
-        <v>769</v>
-      </c>
-      <c r="G250" t="s">
-        <v>759</v>
-      </c>
       <c r="I250" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J250" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M250">
         <v>1</v>
@@ -14640,22 +14640,22 @@
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C251" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D251" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G251" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I251" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J251" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M251">
         <v>1</v>
@@ -14666,22 +14666,22 @@
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C252" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D252" t="s">
+        <v>762</v>
+      </c>
+      <c r="G252" t="s">
         <v>763</v>
       </c>
-      <c r="G252" t="s">
-        <v>764</v>
-      </c>
       <c r="I252" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J252" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M252">
         <v>1</v>
@@ -14692,22 +14692,22 @@
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C253" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D253" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G253" t="s">
+        <v>899</v>
+      </c>
+      <c r="I253" t="s">
+        <v>735</v>
+      </c>
+      <c r="J253" t="s">
         <v>900</v>
-      </c>
-      <c r="I253" t="s">
-        <v>736</v>
-      </c>
-      <c r="J253" t="s">
-        <v>901</v>
       </c>
       <c r="M253">
         <v>1</v>
@@ -14718,22 +14718,22 @@
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C254" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D254" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="G254" t="s">
+        <v>899</v>
+      </c>
+      <c r="I254" t="s">
+        <v>735</v>
+      </c>
+      <c r="J254" t="s">
         <v>900</v>
-      </c>
-      <c r="I254" t="s">
-        <v>736</v>
-      </c>
-      <c r="J254" t="s">
-        <v>901</v>
       </c>
       <c r="M254">
         <v>1</v>
@@ -14744,22 +14744,22 @@
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C255" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D255" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G255" t="s">
+        <v>899</v>
+      </c>
+      <c r="I255" t="s">
+        <v>735</v>
+      </c>
+      <c r="J255" t="s">
         <v>900</v>
-      </c>
-      <c r="I255" t="s">
-        <v>736</v>
-      </c>
-      <c r="J255" t="s">
-        <v>901</v>
       </c>
       <c r="M255">
         <v>1</v>
@@ -14770,22 +14770,22 @@
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C256" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D256" t="s">
+        <v>898</v>
+      </c>
+      <c r="G256" t="s">
         <v>899</v>
       </c>
-      <c r="G256" t="s">
+      <c r="I256" t="s">
+        <v>735</v>
+      </c>
+      <c r="J256" t="s">
         <v>900</v>
-      </c>
-      <c r="I256" t="s">
-        <v>736</v>
-      </c>
-      <c r="J256" t="s">
-        <v>901</v>
       </c>
       <c r="M256">
         <v>1</v>

</xml_diff>